<commit_message>
add Kano model - response
</commit_message>
<xml_diff>
--- a/1-Define/Kano_Model.xlsx
+++ b/1-Define/Kano_Model.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dani_\OneDrive\Documentos\LeanSS\Python\1-Define\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{508552B4-8B96-4C5F-AFDB-9C254D83AD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB7FD52F-B7C6-43C8-B05A-2CA1E1881F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23415" yWindow="0" windowWidth="28290" windowHeight="20985" xr2:uid="{4B24934C-46D6-4CB7-B55D-D582E7CEB4D5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Kano_Model" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -101,11 +101,6 @@
 ¿Cómo te sentirías?</t>
   </si>
   <si>
-    <t>Si no existe la Visualización del 
-pedido vía una app), ¿Cómo te 
-sentirías?</t>
-  </si>
-  <si>
     <t>Si la densidad del casetón es 
 correcta, ¿Cómo te sentirías?</t>
   </si>
@@ -159,6 +154,11 @@
   </si>
   <si>
     <t>Si el casetón no tiene un certificado de calidad, ¿Cómo te sentirías?</t>
+  </si>
+  <si>
+    <t>Si no existe la Visualización del 
+pedido vía una app, ¿Cómo te 
+sentirías?</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:E241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E242" sqref="E242"/>
+      <selection activeCell="C233" sqref="C233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +571,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -585,7 +585,7 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -602,7 +602,7 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -619,7 +619,7 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -633,10 +633,10 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -650,10 +650,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -667,10 +667,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -684,10 +684,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -701,10 +701,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -718,10 +718,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -735,10 +735,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -752,10 +752,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -769,10 +769,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -789,7 +789,7 @@
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -806,7 +806,7 @@
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15">
         <v>5</v>
@@ -823,7 +823,7 @@
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -837,10 +837,10 @@
         <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -854,10 +854,10 @@
         <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -871,10 +871,10 @@
         <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19">
         <v>5</v>
@@ -888,10 +888,10 @@
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -905,10 +905,10 @@
         <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E21">
         <v>3</v>
@@ -922,10 +922,10 @@
         <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -939,10 +939,10 @@
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E23">
         <v>5</v>
@@ -956,10 +956,10 @@
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -973,10 +973,10 @@
         <v>13</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E25">
         <v>3</v>
@@ -993,7 +993,7 @@
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -1010,7 +1010,7 @@
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E27">
         <v>5</v>
@@ -1027,7 +1027,7 @@
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1041,10 +1041,10 @@
         <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E29">
         <v>4</v>
@@ -1058,10 +1058,10 @@
         <v>4</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -1075,10 +1075,10 @@
         <v>9</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E31">
         <v>5</v>
@@ -1092,10 +1092,10 @@
         <v>5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1109,10 +1109,10 @@
         <v>11</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E33">
         <v>3</v>
@@ -1126,10 +1126,10 @@
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E34">
         <v>3</v>
@@ -1143,10 +1143,10 @@
         <v>12</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E35">
         <v>5</v>
@@ -1160,10 +1160,10 @@
         <v>7</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E36">
         <v>3</v>
@@ -1177,10 +1177,10 @@
         <v>13</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -1197,7 +1197,7 @@
         <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -1214,7 +1214,7 @@
         <v>17</v>
       </c>
       <c r="D39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E39">
         <v>5</v>
@@ -1231,7 +1231,7 @@
         <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1245,10 +1245,10 @@
         <v>10</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -1262,10 +1262,10 @@
         <v>4</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -1279,10 +1279,10 @@
         <v>9</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E43">
         <v>5</v>
@@ -1296,10 +1296,10 @@
         <v>5</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -1313,10 +1313,10 @@
         <v>11</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E45">
         <v>3</v>
@@ -1330,10 +1330,10 @@
         <v>6</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E46">
         <v>2</v>
@@ -1347,10 +1347,10 @@
         <v>12</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E47">
         <v>5</v>
@@ -1364,10 +1364,10 @@
         <v>7</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E48">
         <v>3</v>
@@ -1381,10 +1381,10 @@
         <v>13</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E49">
         <v>3</v>
@@ -1401,7 +1401,7 @@
         <v>16</v>
       </c>
       <c r="D50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -1418,7 +1418,7 @@
         <v>17</v>
       </c>
       <c r="D51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E51">
         <v>5</v>
@@ -1435,7 +1435,7 @@
         <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -1449,10 +1449,10 @@
         <v>10</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E53">
         <v>4</v>
@@ -1466,10 +1466,10 @@
         <v>4</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E54">
         <v>2</v>
@@ -1483,10 +1483,10 @@
         <v>9</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E55">
         <v>5</v>
@@ -1500,10 +1500,10 @@
         <v>5</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D56" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -1517,10 +1517,10 @@
         <v>11</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E57">
         <v>3</v>
@@ -1534,10 +1534,10 @@
         <v>6</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D58" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E58">
         <v>2</v>
@@ -1551,10 +1551,10 @@
         <v>12</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D59" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E59">
         <v>5</v>
@@ -1568,10 +1568,10 @@
         <v>7</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E60">
         <v>3</v>
@@ -1585,10 +1585,10 @@
         <v>13</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D61" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E61">
         <v>4</v>
@@ -1605,7 +1605,7 @@
         <v>16</v>
       </c>
       <c r="D62" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -1622,7 +1622,7 @@
         <v>17</v>
       </c>
       <c r="D63" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E63">
         <v>5</v>
@@ -1639,7 +1639,7 @@
         <v>18</v>
       </c>
       <c r="D64" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -1653,10 +1653,10 @@
         <v>10</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E65">
         <v>4</v>
@@ -1670,10 +1670,10 @@
         <v>4</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E66">
         <v>3</v>
@@ -1687,10 +1687,10 @@
         <v>9</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D67" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E67">
         <v>4</v>
@@ -1704,10 +1704,10 @@
         <v>5</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D68" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -1721,10 +1721,10 @@
         <v>11</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D69" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E69">
         <v>3</v>
@@ -1738,10 +1738,10 @@
         <v>6</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D70" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E70">
         <v>3</v>
@@ -1755,10 +1755,10 @@
         <v>12</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E71">
         <v>3</v>
@@ -1772,10 +1772,10 @@
         <v>7</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D72" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E72">
         <v>3</v>
@@ -1789,10 +1789,10 @@
         <v>13</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D73" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E73">
         <v>4</v>
@@ -1809,7 +1809,7 @@
         <v>16</v>
       </c>
       <c r="D74" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E74">
         <v>1</v>
@@ -1826,7 +1826,7 @@
         <v>17</v>
       </c>
       <c r="D75" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E75">
         <v>5</v>
@@ -1843,7 +1843,7 @@
         <v>18</v>
       </c>
       <c r="D76" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -1857,10 +1857,10 @@
         <v>10</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D77" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E77">
         <v>4</v>
@@ -1874,10 +1874,10 @@
         <v>4</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D78" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E78">
         <v>3</v>
@@ -1891,10 +1891,10 @@
         <v>9</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D79" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E79">
         <v>4</v>
@@ -1908,10 +1908,10 @@
         <v>5</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D80" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -1925,10 +1925,10 @@
         <v>11</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D81" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E81">
         <v>3</v>
@@ -1942,10 +1942,10 @@
         <v>6</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D82" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E82">
         <v>3</v>
@@ -1959,10 +1959,10 @@
         <v>12</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D83" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E83">
         <v>3</v>
@@ -1976,10 +1976,10 @@
         <v>7</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D84" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E84">
         <v>5</v>
@@ -1993,10 +1993,10 @@
         <v>13</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D85" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E85">
         <v>4</v>
@@ -2013,7 +2013,7 @@
         <v>16</v>
       </c>
       <c r="D86" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E86">
         <v>2</v>
@@ -2030,7 +2030,7 @@
         <v>17</v>
       </c>
       <c r="D87" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E87">
         <v>5</v>
@@ -2047,7 +2047,7 @@
         <v>18</v>
       </c>
       <c r="D88" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -2061,10 +2061,10 @@
         <v>10</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D89" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E89">
         <v>4</v>
@@ -2078,10 +2078,10 @@
         <v>4</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D90" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E90">
         <v>2</v>
@@ -2095,10 +2095,10 @@
         <v>9</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D91" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E91">
         <v>5</v>
@@ -2112,10 +2112,10 @@
         <v>5</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D92" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -2129,10 +2129,10 @@
         <v>11</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D93" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E93">
         <v>4</v>
@@ -2146,10 +2146,10 @@
         <v>6</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D94" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E94">
         <v>3</v>
@@ -2163,10 +2163,10 @@
         <v>12</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D95" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E95">
         <v>3</v>
@@ -2180,10 +2180,10 @@
         <v>7</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D96" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E96">
         <v>3</v>
@@ -2197,10 +2197,10 @@
         <v>13</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E97">
         <v>3</v>
@@ -2217,7 +2217,7 @@
         <v>16</v>
       </c>
       <c r="D98" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E98">
         <v>2</v>
@@ -2234,7 +2234,7 @@
         <v>17</v>
       </c>
       <c r="D99" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E99">
         <v>5</v>
@@ -2251,7 +2251,7 @@
         <v>18</v>
       </c>
       <c r="D100" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -2265,10 +2265,10 @@
         <v>10</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D101" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E101">
         <v>4</v>
@@ -2282,10 +2282,10 @@
         <v>4</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D102" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E102">
         <v>2</v>
@@ -2299,10 +2299,10 @@
         <v>9</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D103" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E103">
         <v>5</v>
@@ -2316,10 +2316,10 @@
         <v>5</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D104" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E104">
         <v>1</v>
@@ -2333,10 +2333,10 @@
         <v>11</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D105" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E105">
         <v>4</v>
@@ -2350,10 +2350,10 @@
         <v>6</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D106" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E106">
         <v>3</v>
@@ -2367,10 +2367,10 @@
         <v>12</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D107" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E107">
         <v>3</v>
@@ -2384,10 +2384,10 @@
         <v>7</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D108" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E108">
         <v>3</v>
@@ -2401,10 +2401,10 @@
         <v>13</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D109" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E109">
         <v>3</v>
@@ -2421,7 +2421,7 @@
         <v>16</v>
       </c>
       <c r="D110" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E110">
         <v>2</v>
@@ -2438,7 +2438,7 @@
         <v>17</v>
       </c>
       <c r="D111" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E111">
         <v>5</v>
@@ -2455,7 +2455,7 @@
         <v>18</v>
       </c>
       <c r="D112" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -2469,10 +2469,10 @@
         <v>10</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D113" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E113">
         <v>4</v>
@@ -2486,10 +2486,10 @@
         <v>4</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D114" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E114">
         <v>2</v>
@@ -2503,10 +2503,10 @@
         <v>9</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D115" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E115">
         <v>5</v>
@@ -2520,10 +2520,10 @@
         <v>5</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D116" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E116">
         <v>1</v>
@@ -2537,10 +2537,10 @@
         <v>11</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D117" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E117">
         <v>4</v>
@@ -2554,10 +2554,10 @@
         <v>6</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D118" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E118">
         <v>3</v>
@@ -2571,10 +2571,10 @@
         <v>12</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D119" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E119">
         <v>3</v>
@@ -2588,10 +2588,10 @@
         <v>7</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D120" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E120">
         <v>3</v>
@@ -2605,10 +2605,10 @@
         <v>13</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D121" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E121">
         <v>3</v>
@@ -2625,7 +2625,7 @@
         <v>16</v>
       </c>
       <c r="D122" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E122">
         <v>2</v>
@@ -2642,7 +2642,7 @@
         <v>17</v>
       </c>
       <c r="D123" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E123">
         <v>5</v>
@@ -2659,7 +2659,7 @@
         <v>18</v>
       </c>
       <c r="D124" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E124">
         <v>1</v>
@@ -2673,10 +2673,10 @@
         <v>10</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D125" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E125">
         <v>4</v>
@@ -2690,10 +2690,10 @@
         <v>4</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D126" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E126">
         <v>2</v>
@@ -2707,10 +2707,10 @@
         <v>9</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D127" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E127">
         <v>5</v>
@@ -2724,10 +2724,10 @@
         <v>5</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D128" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E128">
         <v>1</v>
@@ -2741,10 +2741,10 @@
         <v>11</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D129" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E129">
         <v>4</v>
@@ -2758,10 +2758,10 @@
         <v>6</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D130" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E130">
         <v>3</v>
@@ -2775,10 +2775,10 @@
         <v>12</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D131" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E131">
         <v>3</v>
@@ -2792,10 +2792,10 @@
         <v>7</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D132" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E132">
         <v>3</v>
@@ -2809,10 +2809,10 @@
         <v>13</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D133" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E133">
         <v>3</v>
@@ -2829,7 +2829,7 @@
         <v>16</v>
       </c>
       <c r="D134" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E134">
         <v>2</v>
@@ -2846,7 +2846,7 @@
         <v>17</v>
       </c>
       <c r="D135" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E135">
         <v>5</v>
@@ -2863,7 +2863,7 @@
         <v>18</v>
       </c>
       <c r="D136" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E136">
         <v>1</v>
@@ -2877,10 +2877,10 @@
         <v>10</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D137" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E137">
         <v>4</v>
@@ -2894,10 +2894,10 @@
         <v>4</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D138" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E138">
         <v>2</v>
@@ -2911,10 +2911,10 @@
         <v>9</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D139" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E139">
         <v>5</v>
@@ -2928,10 +2928,10 @@
         <v>5</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D140" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E140">
         <v>1</v>
@@ -2945,10 +2945,10 @@
         <v>11</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D141" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E141">
         <v>4</v>
@@ -2962,10 +2962,10 @@
         <v>6</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D142" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E142">
         <v>3</v>
@@ -2979,10 +2979,10 @@
         <v>12</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D143" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E143">
         <v>3</v>
@@ -2996,10 +2996,10 @@
         <v>7</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D144" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E144">
         <v>3</v>
@@ -3013,10 +3013,10 @@
         <v>13</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D145" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E145">
         <v>3</v>
@@ -3033,7 +3033,7 @@
         <v>16</v>
       </c>
       <c r="D146" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E146">
         <v>2</v>
@@ -3050,7 +3050,7 @@
         <v>17</v>
       </c>
       <c r="D147" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E147">
         <v>5</v>
@@ -3067,7 +3067,7 @@
         <v>18</v>
       </c>
       <c r="D148" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E148">
         <v>1</v>
@@ -3081,10 +3081,10 @@
         <v>10</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D149" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E149">
         <v>4</v>
@@ -3098,10 +3098,10 @@
         <v>4</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D150" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E150">
         <v>2</v>
@@ -3115,10 +3115,10 @@
         <v>9</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D151" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E151">
         <v>5</v>
@@ -3132,10 +3132,10 @@
         <v>5</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D152" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E152">
         <v>1</v>
@@ -3149,10 +3149,10 @@
         <v>11</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D153" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E153">
         <v>4</v>
@@ -3166,10 +3166,10 @@
         <v>6</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D154" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E154">
         <v>3</v>
@@ -3183,10 +3183,10 @@
         <v>12</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D155" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E155">
         <v>3</v>
@@ -3200,10 +3200,10 @@
         <v>7</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D156" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E156">
         <v>3</v>
@@ -3217,10 +3217,10 @@
         <v>13</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D157" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E157">
         <v>3</v>
@@ -3237,7 +3237,7 @@
         <v>16</v>
       </c>
       <c r="D158" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E158">
         <v>2</v>
@@ -3254,7 +3254,7 @@
         <v>17</v>
       </c>
       <c r="D159" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E159">
         <v>5</v>
@@ -3271,7 +3271,7 @@
         <v>18</v>
       </c>
       <c r="D160" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E160">
         <v>1</v>
@@ -3285,10 +3285,10 @@
         <v>10</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D161" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E161">
         <v>4</v>
@@ -3302,10 +3302,10 @@
         <v>4</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D162" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E162">
         <v>2</v>
@@ -3319,10 +3319,10 @@
         <v>9</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D163" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E163">
         <v>5</v>
@@ -3336,10 +3336,10 @@
         <v>5</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D164" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E164">
         <v>1</v>
@@ -3353,10 +3353,10 @@
         <v>11</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D165" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E165">
         <v>4</v>
@@ -3370,10 +3370,10 @@
         <v>6</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D166" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E166">
         <v>3</v>
@@ -3387,10 +3387,10 @@
         <v>12</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D167" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E167">
         <v>3</v>
@@ -3404,10 +3404,10 @@
         <v>7</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D168" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E168">
         <v>3</v>
@@ -3421,10 +3421,10 @@
         <v>13</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D169" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E169">
         <v>3</v>
@@ -3441,7 +3441,7 @@
         <v>16</v>
       </c>
       <c r="D170" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E170">
         <v>2</v>
@@ -3458,7 +3458,7 @@
         <v>17</v>
       </c>
       <c r="D171" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E171">
         <v>5</v>
@@ -3475,7 +3475,7 @@
         <v>18</v>
       </c>
       <c r="D172" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E172">
         <v>1</v>
@@ -3489,10 +3489,10 @@
         <v>10</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D173" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E173">
         <v>4</v>
@@ -3506,10 +3506,10 @@
         <v>4</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D174" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E174">
         <v>2</v>
@@ -3523,10 +3523,10 @@
         <v>9</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D175" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E175">
         <v>5</v>
@@ -3540,10 +3540,10 @@
         <v>5</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D176" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E176">
         <v>1</v>
@@ -3557,10 +3557,10 @@
         <v>11</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D177" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E177">
         <v>4</v>
@@ -3574,10 +3574,10 @@
         <v>6</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D178" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E178">
         <v>3</v>
@@ -3591,10 +3591,10 @@
         <v>12</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D179" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E179">
         <v>3</v>
@@ -3608,10 +3608,10 @@
         <v>7</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D180" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E180">
         <v>3</v>
@@ -3625,10 +3625,10 @@
         <v>13</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D181" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E181">
         <v>3</v>
@@ -3645,7 +3645,7 @@
         <v>16</v>
       </c>
       <c r="D182" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E182">
         <v>2</v>
@@ -3662,7 +3662,7 @@
         <v>17</v>
       </c>
       <c r="D183" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E183">
         <v>5</v>
@@ -3679,7 +3679,7 @@
         <v>18</v>
       </c>
       <c r="D184" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E184">
         <v>1</v>
@@ -3693,10 +3693,10 @@
         <v>10</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D185" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E185">
         <v>4</v>
@@ -3710,10 +3710,10 @@
         <v>4</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D186" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E186">
         <v>2</v>
@@ -3727,10 +3727,10 @@
         <v>9</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D187" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E187">
         <v>5</v>
@@ -3744,10 +3744,10 @@
         <v>5</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D188" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E188">
         <v>1</v>
@@ -3761,10 +3761,10 @@
         <v>11</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D189" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E189">
         <v>4</v>
@@ -3778,10 +3778,10 @@
         <v>6</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D190" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E190">
         <v>3</v>
@@ -3795,10 +3795,10 @@
         <v>12</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D191" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E191">
         <v>3</v>
@@ -3812,10 +3812,10 @@
         <v>7</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D192" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E192">
         <v>3</v>
@@ -3829,10 +3829,10 @@
         <v>13</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D193" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E193">
         <v>3</v>
@@ -3849,7 +3849,7 @@
         <v>16</v>
       </c>
       <c r="D194" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E194">
         <v>2</v>
@@ -3866,7 +3866,7 @@
         <v>17</v>
       </c>
       <c r="D195" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E195">
         <v>5</v>
@@ -3883,7 +3883,7 @@
         <v>18</v>
       </c>
       <c r="D196" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E196">
         <v>1</v>
@@ -3897,10 +3897,10 @@
         <v>10</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D197" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E197">
         <v>4</v>
@@ -3914,10 +3914,10 @@
         <v>4</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D198" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E198">
         <v>2</v>
@@ -3931,10 +3931,10 @@
         <v>9</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D199" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E199">
         <v>5</v>
@@ -3948,10 +3948,10 @@
         <v>5</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D200" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E200">
         <v>1</v>
@@ -3965,10 +3965,10 @@
         <v>11</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D201" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E201">
         <v>4</v>
@@ -3982,10 +3982,10 @@
         <v>6</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D202" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E202">
         <v>3</v>
@@ -3999,10 +3999,10 @@
         <v>12</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D203" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E203">
         <v>3</v>
@@ -4016,10 +4016,10 @@
         <v>7</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D204" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E204">
         <v>3</v>
@@ -4033,10 +4033,10 @@
         <v>13</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D205" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E205">
         <v>3</v>
@@ -4053,7 +4053,7 @@
         <v>16</v>
       </c>
       <c r="D206" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E206">
         <v>2</v>
@@ -4070,7 +4070,7 @@
         <v>17</v>
       </c>
       <c r="D207" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E207">
         <v>5</v>
@@ -4087,7 +4087,7 @@
         <v>18</v>
       </c>
       <c r="D208" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E208">
         <v>1</v>
@@ -4101,10 +4101,10 @@
         <v>10</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D209" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E209">
         <v>4</v>
@@ -4118,10 +4118,10 @@
         <v>4</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D210" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E210">
         <v>2</v>
@@ -4135,10 +4135,10 @@
         <v>9</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D211" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E211">
         <v>5</v>
@@ -4152,10 +4152,10 @@
         <v>5</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D212" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E212">
         <v>1</v>
@@ -4169,10 +4169,10 @@
         <v>11</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D213" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E213">
         <v>4</v>
@@ -4186,10 +4186,10 @@
         <v>6</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D214" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E214">
         <v>2</v>
@@ -4203,10 +4203,10 @@
         <v>12</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D215" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E215">
         <v>5</v>
@@ -4220,10 +4220,10 @@
         <v>7</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D216" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E216">
         <v>3</v>
@@ -4237,10 +4237,10 @@
         <v>13</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D217" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E217">
         <v>3</v>
@@ -4257,7 +4257,7 @@
         <v>16</v>
       </c>
       <c r="D218" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E218">
         <v>2</v>
@@ -4274,7 +4274,7 @@
         <v>17</v>
       </c>
       <c r="D219" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E219">
         <v>5</v>
@@ -4291,7 +4291,7 @@
         <v>18</v>
       </c>
       <c r="D220" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E220">
         <v>1</v>
@@ -4305,10 +4305,10 @@
         <v>10</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D221" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E221">
         <v>4</v>
@@ -4322,10 +4322,10 @@
         <v>4</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D222" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E222">
         <v>2</v>
@@ -4339,10 +4339,10 @@
         <v>9</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D223" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E223">
         <v>5</v>
@@ -4356,10 +4356,10 @@
         <v>5</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D224" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E224">
         <v>1</v>
@@ -4373,10 +4373,10 @@
         <v>11</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D225" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E225">
         <v>4</v>
@@ -4390,10 +4390,10 @@
         <v>6</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D226" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E226">
         <v>2</v>
@@ -4407,10 +4407,10 @@
         <v>12</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D227" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E227">
         <v>5</v>
@@ -4424,10 +4424,10 @@
         <v>7</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D228" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E228">
         <v>5</v>
@@ -4441,10 +4441,10 @@
         <v>13</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D229" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E229">
         <v>1</v>
@@ -4461,7 +4461,7 @@
         <v>16</v>
       </c>
       <c r="D230" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E230">
         <v>2</v>
@@ -4478,7 +4478,7 @@
         <v>17</v>
       </c>
       <c r="D231" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E231">
         <v>5</v>
@@ -4495,7 +4495,7 @@
         <v>18</v>
       </c>
       <c r="D232" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E232">
         <v>1</v>
@@ -4509,10 +4509,10 @@
         <v>10</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D233" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E233">
         <v>4</v>
@@ -4526,10 +4526,10 @@
         <v>4</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D234" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E234">
         <v>2</v>
@@ -4543,10 +4543,10 @@
         <v>9</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D235" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E235">
         <v>5</v>
@@ -4560,10 +4560,10 @@
         <v>5</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D236" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E236">
         <v>1</v>
@@ -4577,10 +4577,10 @@
         <v>11</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D237" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E237">
         <v>4</v>
@@ -4594,10 +4594,10 @@
         <v>6</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D238" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E238">
         <v>2</v>
@@ -4611,10 +4611,10 @@
         <v>12</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D239" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E239">
         <v>5</v>
@@ -4628,10 +4628,10 @@
         <v>7</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D240" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E240">
         <v>1</v>
@@ -4645,10 +4645,10 @@
         <v>13</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D241" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E241">
         <v>1</v>

</xml_diff>